<commit_message>
combine all solutions in one folder
</commit_message>
<xml_diff>
--- a/record.xlsx
+++ b/record.xlsx
@@ -1,36 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylexiao/Documents/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2BDDA5-BEF3-7548-A29B-EF451127D106}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="28000" windowHeight="17540"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="31700" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="41">
   <si>
     <t>Week</t>
   </si>
@@ -80,15 +81,6 @@
     <t>23/4/18</t>
   </si>
   <si>
-    <t>there are 60 questions of medium by top 300</t>
-  </si>
-  <si>
-    <t>finish 10 by this week</t>
-  </si>
-  <si>
-    <t>finish the rest 50 by next 2 week</t>
-  </si>
-  <si>
     <t>REVIEW</t>
   </si>
   <si>
@@ -105,12 +97,69 @@
   </si>
   <si>
     <t>2. backtrack vs dfs</t>
+  </si>
+  <si>
+    <t>Plan for the next 3 weeks</t>
+  </si>
+  <si>
+    <t>week 1</t>
+  </si>
+  <si>
+    <t>week 2</t>
+  </si>
+  <si>
+    <t>week 3</t>
+  </si>
+  <si>
+    <t>Plan for the rest 4 weeks</t>
+  </si>
+  <si>
+    <t>week 4</t>
+  </si>
+  <si>
+    <t>复习1-150</t>
+  </si>
+  <si>
+    <t>复习151-300</t>
+  </si>
+  <si>
+    <t>复习300-400, 三刷1-100</t>
+  </si>
+  <si>
+    <t>三刷101-300</t>
+  </si>
+  <si>
+    <t>在家10天</t>
+  </si>
+  <si>
+    <t>三刷301-400</t>
+  </si>
+  <si>
+    <t>average daily</t>
+  </si>
+  <si>
+    <t>完成度</t>
+  </si>
+  <si>
+    <t>完成了35</t>
+  </si>
+  <si>
+    <t>完成前400</t>
+  </si>
+  <si>
+    <t>每天必须要做5道hard</t>
+  </si>
+  <si>
+    <t>剩下5道medium</t>
+  </si>
+  <si>
+    <t>&lt;- sql题 暂时忽略</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -127,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +186,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,12 +214,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,11 +536,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="136" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -489,8 +553,9 @@
     <col min="6" max="6" width="10.83203125" style="2"/>
     <col min="7" max="7" width="63" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -523,23 +588,23 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2">
         <f>SUM(C4:C1111)</f>
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(D4:D1111)</f>
-        <v>119</v>
+        <v>193</v>
       </c>
       <c r="E3" s="2">
         <f xml:space="preserve"> SUM(E4:E1111)</f>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2">
-        <f xml:space="preserve"> SUM(C3:E3)</f>
-        <v>189</v>
+        <f>SUM(C3:E3,F5,F4)</f>
+        <v>332</v>
       </c>
       <c r="G3" s="1">
         <f xml:space="preserve"> F3/808 %</f>
-        <v>23.39108910891089</v>
+        <v>41.089108910891092</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -562,6 +627,12 @@
       </c>
       <c r="C5" s="1">
         <v>11</v>
+      </c>
+      <c r="F5" s="2">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -869,7 +940,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -927,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -958,7 +1029,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1103,7 +1174,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>12</v>
@@ -1116,13 +1187,13 @@
         <v>24</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -1135,9 +1206,7 @@
       <c r="D76" s="1">
         <v>5</v>
       </c>
-      <c r="G76" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="G76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
@@ -1149,9 +1218,7 @@
       <c r="D77" s="1">
         <v>3</v>
       </c>
-      <c r="G77" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
@@ -1160,9 +1227,7 @@
       <c r="D78" s="1">
         <v>5</v>
       </c>
-      <c r="G78" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="G78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
@@ -1180,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
         <v>11</v>
       </c>
@@ -1188,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
         <v>12</v>
       </c>
@@ -1198,6 +1263,346 @@
       <c r="F82" s="2">
         <f>SUM(C76:E82)</f>
         <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="6">
+        <v>11</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6">
+        <v>6</v>
+      </c>
+      <c r="E84" s="6"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="7">
+        <v>43262</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6">
+        <v>5</v>
+      </c>
+      <c r="E85" s="6"/>
+      <c r="H85" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I85" s="5">
+        <v>40</v>
+      </c>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="6">
+        <v>2</v>
+      </c>
+      <c r="D86" s="6">
+        <v>8</v>
+      </c>
+      <c r="E86" s="6"/>
+      <c r="H86" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I86" s="5">
+        <v>75</v>
+      </c>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="6"/>
+      <c r="B87" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="6">
+        <v>1</v>
+      </c>
+      <c r="D87" s="6">
+        <v>9</v>
+      </c>
+      <c r="E87" s="6"/>
+      <c r="H87" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I87" s="5">
+        <v>75</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K87" s="5"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" s="6"/>
+      <c r="B88" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="6">
+        <v>1</v>
+      </c>
+      <c r="D88" s="6">
+        <v>4</v>
+      </c>
+      <c r="E88" s="6"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" s="6"/>
+      <c r="B89" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" s="6">
+        <v>5</v>
+      </c>
+      <c r="D89" s="6">
+        <v>5</v>
+      </c>
+      <c r="E89" s="6"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K89" s="5"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="6"/>
+      <c r="B90" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" s="6">
+        <v>3</v>
+      </c>
+      <c r="D90" s="6">
+        <v>2</v>
+      </c>
+      <c r="E90" s="6">
+        <v>5</v>
+      </c>
+      <c r="F90" s="2">
+        <f>SUM(C84:E90)</f>
+        <v>56</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J90" s="5">
+        <v>21</v>
+      </c>
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H91" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J91" s="5">
+        <v>21</v>
+      </c>
+      <c r="K91" s="5"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>12</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92" s="1">
+        <v>5</v>
+      </c>
+      <c r="E92" s="1">
+        <v>5</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J92" s="5">
+        <v>28</v>
+      </c>
+      <c r="K92" s="5"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <v>43269</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="1">
+        <v>6</v>
+      </c>
+      <c r="D93" s="1">
+        <v>3</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J93" s="5">
+        <v>28</v>
+      </c>
+      <c r="K93" s="5"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="1">
+        <v>3</v>
+      </c>
+      <c r="D94" s="1">
+        <v>4</v>
+      </c>
+      <c r="E94" s="1">
+        <v>3</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J94" s="5">
+        <v>10</v>
+      </c>
+      <c r="K94" s="5"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" s="1">
+        <v>8</v>
+      </c>
+      <c r="E96" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="1">
+        <v>2</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1</v>
+      </c>
+      <c r="F98" s="2">
+        <f>SUM(C92:E98)</f>
+        <v>58</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G99" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>12</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="3">
+        <v>43276</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B102" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B103" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B104" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B105" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106" s="2">
+        <f>SUM(C100:E106)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>